<commit_message>
Tweak shift parameter to use Python output
</commit_message>
<xml_diff>
--- a/data/ons_weekly_deaths_2020.xlsx
+++ b/data/ons_weekly_deaths_2020.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\WCA\ons-stats\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE447922-6B3E-4208-B28D-BFF0D7D007FE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AAB7A10-D4E8-4638-8E1D-0C8F8CFCDAA2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="748" activeTab="9" xr2:uid="{2E10C76F-872B-452C-8A27-924470753E43}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="47">
   <si>
     <t>Week number</t>
   </si>
@@ -177,6 +177,12 @@
   </si>
   <si>
     <t>EXCESS DEATHS - 20 Mar to 12 Jun</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Only used for demo purposes!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Derived by Python notebook called "determine_shift_params" </t>
   </si>
 </sst>
 </file>
@@ -1119,7 +1125,6 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="3" fontId="22" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="3" fontId="23" fillId="5" borderId="0" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="23" fillId="5" borderId="0" xfId="19" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
@@ -1132,6 +1137,7 @@
     <xf numFmtId="3" fontId="2" fillId="4" borderId="0" xfId="19" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="3" fontId="22" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="502">
     <cellStyle name="Comma 10" xfId="2" xr:uid="{2FBB2085-3E13-40B4-82E9-34FA0C408571}"/>
@@ -1685,7 +1691,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-GB"/>
-              <a:t>Daily death occurences where COVID-19 was mentioned on the death certificate</a:t>
+              <a:t>Daily death occurrences where COVID-19 was mentioned on the death certificate</a:t>
             </a:r>
           </a:p>
           <a:p>
@@ -3725,61 +3731,61 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="19"/>
                 <c:pt idx="0">
-                  <c:v>10946</c:v>
+                  <c:v>10958.07</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10811.714285714286</c:v>
+                  <c:v>10763.84</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10567.714285714286</c:v>
+                  <c:v>10573.8</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>11592</c:v>
+                  <c:v>11826.3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>13239.642857142857</c:v>
+                  <c:v>13317.184999999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>13712.285714285714</c:v>
+                  <c:v>13720.755000000001</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>13319.857142857141</c:v>
+                  <c:v>13215.69</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>12163.642857142859</c:v>
+                  <c:v>12028.895</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>11003.714285714286</c:v>
+                  <c:v>10908.861666666668</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>10097.380952380952</c:v>
+                  <c:v>10009.352222222224</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>9394.3492063492067</c:v>
+                  <c:v>9345.3366666666661</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>8941.5555555555566</c:v>
+                  <c:v>8899.7444444444445</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>8682.7142857142844</c:v>
+                  <c:v>8677.2033333333329</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>8641.2380952380954</c:v>
+                  <c:v>8638.77</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>8596.7619047619046</c:v>
+                  <c:v>8589.5266666666666</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>8477.5714285714275</c:v>
+                  <c:v>8459.01</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>8473.7142857142862</c:v>
+                  <c:v>8497.5499999999993</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>8486.2857142857138</c:v>
+                  <c:v>8457.48</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>8411.4285714285725</c:v>
+                  <c:v>8432.119999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4336,61 +4342,61 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="19"/>
                 <c:pt idx="0">
-                  <c:v>10952</c:v>
+                  <c:v>10964.07</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10855.714285714286</c:v>
+                  <c:v>10807.84</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10968.714285714286</c:v>
+                  <c:v>10974.8</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>13463</c:v>
+                  <c:v>13697.3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>18411.642857142855</c:v>
+                  <c:v>18489.184999999998</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>21926.285714285714</c:v>
+                  <c:v>21934.755000000001</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>21609.857142857141</c:v>
+                  <c:v>21505.690000000002</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>19078.642857142859</c:v>
+                  <c:v>18943.895</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>16187.714285714286</c:v>
+                  <c:v>16092.861666666668</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>14064.380952380952</c:v>
+                  <c:v>13976.352222222224</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>12245.349206349207</c:v>
+                  <c:v>12196.336666666666</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>11208.555555555557</c:v>
+                  <c:v>11166.744444444445</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>10452.714285714284</c:v>
+                  <c:v>10447.203333333333</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>9940.2380952380954</c:v>
+                  <c:v>9937.77</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>9531.7619047619046</c:v>
+                  <c:v>9524.5266666666666</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>9148.5714285714275</c:v>
+                  <c:v>9130.01</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>9045.7142857142862</c:v>
+                  <c:v>9069.5499999999993</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>8908.2857142857138</c:v>
+                  <c:v>8879.48</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>8734.4285714285725</c:v>
+                  <c:v>8755.119999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5263,61 +5269,61 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="19"/>
                 <c:pt idx="0">
-                  <c:v>10952</c:v>
+                  <c:v>10964.07</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10855.714285714286</c:v>
+                  <c:v>10807.84</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10968.714285714286</c:v>
+                  <c:v>10974.8</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>13463</c:v>
+                  <c:v>13697.3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>18411.642857142855</c:v>
+                  <c:v>18489.184999999998</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>21926.285714285714</c:v>
+                  <c:v>21934.755000000001</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>21609.857142857141</c:v>
+                  <c:v>21505.690000000002</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>19078.642857142859</c:v>
+                  <c:v>18943.895</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>16187.714285714286</c:v>
+                  <c:v>16092.861666666668</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>14064.380952380952</c:v>
+                  <c:v>13976.352222222224</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>12245.349206349207</c:v>
+                  <c:v>12196.336666666666</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>11208.555555555557</c:v>
+                  <c:v>11166.744444444445</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>10452.714285714284</c:v>
+                  <c:v>10447.203333333333</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>9940.2380952380954</c:v>
+                  <c:v>9937.77</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>9531.7619047619046</c:v>
+                  <c:v>9524.5266666666666</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>9148.5714285714275</c:v>
+                  <c:v>9130.01</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>9045.7142857142862</c:v>
+                  <c:v>9069.5499999999993</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>8908.2857142857138</c:v>
+                  <c:v>8879.48</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>8734.4285714285725</c:v>
+                  <c:v>8755.119999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6058,88 +6064,88 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="28"/>
                 <c:pt idx="0">
-                  <c:v>13027.142857142857</c:v>
+                  <c:v>13210.12</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>13600.285714285714</c:v>
+                  <c:v>13491.96</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>12504</c:v>
+                  <c:v>12388.98</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>11751.428571428572</c:v>
+                  <c:v>11726.68</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>11343.714285714286</c:v>
+                  <c:v>11280.22</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>10968</c:v>
+                  <c:v>10963.740000000002</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>10899.857142857143</c:v>
+                  <c:v>10889.41</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>10830.285714285714</c:v>
+                  <c:v>10827.75</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>10849.857142857143</c:v>
+                  <c:v>10857.869999999999</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>10952</c:v>
+                  <c:v>10964.07</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>10855.714285714286</c:v>
+                  <c:v>10807.84</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>10968.714285714286</c:v>
+                  <c:v>10974.8</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>13463</c:v>
+                  <c:v>13697.3</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>18411.642857142855</c:v>
+                  <c:v>18489.184999999998</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>21926.285714285714</c:v>
+                  <c:v>21934.755000000001</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>21609.857142857141</c:v>
+                  <c:v>21505.690000000002</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>19078.642857142859</c:v>
+                  <c:v>18943.895</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>16187.714285714286</c:v>
+                  <c:v>16092.861666666668</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>14064.380952380952</c:v>
+                  <c:v>13976.352222222224</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>12245.349206349207</c:v>
+                  <c:v>12196.336666666666</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>11208.555555555557</c:v>
+                  <c:v>11166.744444444445</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>10452.714285714284</c:v>
+                  <c:v>10447.203333333333</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>9940.2380952380954</c:v>
+                  <c:v>9937.77</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>9531.7619047619046</c:v>
+                  <c:v>9524.5266666666666</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>9148.5714285714275</c:v>
+                  <c:v>9130.01</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>9045.7142857142862</c:v>
+                  <c:v>9069.5499999999993</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>8908.2857142857138</c:v>
+                  <c:v>8879.48</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>8734.4285714285725</c:v>
+                  <c:v>8755.119999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -11238,6 +11244,7 @@
         <c:axId val="693275184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="9000"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -12348,61 +12355,61 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="19"/>
                 <c:pt idx="0">
-                  <c:v>2.1428571428571432</c:v>
+                  <c:v>2.6500000000000004</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>47</c:v>
+                  <c:v>56.940000000000005</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>289.85714285714289</c:v>
+                  <c:v>334.08000000000004</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1797.2857142857144</c:v>
+                  <c:v>2095.08</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4648.4285714285716</c:v>
+                  <c:v>4926.1400000000003</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>7303.7142857142862</c:v>
+                  <c:v>7561.8499999999995</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>8534.7142857142862</c:v>
+                  <c:v>8481.8700000000008</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>7293.2857142857138</c:v>
+                  <c:v>7069.9400000000005</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>5132.8571428571431</c:v>
+                  <c:v>4919.3500000000004</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3878.5714285714284</c:v>
+                  <c:v>3866.4</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3286.7142857142853</c:v>
+                  <c:v>3162.87</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2260.2857142857142</c:v>
+                  <c:v>2182.4899999999998</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1721.7142857142858</c:v>
+                  <c:v>1697.98</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1384.8571428571427</c:v>
+                  <c:v>1336.7800000000002</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>972.14285714285711</c:v>
+                  <c:v>938.56999999999994</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>707.14285714285711</c:v>
+                  <c:v>689.19</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>574.28571428571433</c:v>
+                  <c:v>566.78</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>460.85714285714289</c:v>
+                  <c:v>444.02</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>335.57142857142856</c:v>
+                  <c:v>328.37</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -14072,61 +14079,61 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="19"/>
                 <c:pt idx="0">
-                  <c:v>10946</c:v>
+                  <c:v>10958.07</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10811.714285714286</c:v>
+                  <c:v>10763.84</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10567.714285714286</c:v>
+                  <c:v>10573.8</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>11592</c:v>
+                  <c:v>11826.3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>13239.642857142857</c:v>
+                  <c:v>13317.184999999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>13712.285714285714</c:v>
+                  <c:v>13720.755000000001</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>13319.857142857141</c:v>
+                  <c:v>13215.69</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>12163.642857142859</c:v>
+                  <c:v>12028.895</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>11003.714285714286</c:v>
+                  <c:v>10908.861666666668</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>10097.380952380952</c:v>
+                  <c:v>10009.352222222224</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>9394.3492063492067</c:v>
+                  <c:v>9345.3366666666661</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>8941.5555555555566</c:v>
+                  <c:v>8899.7444444444445</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>8682.7142857142844</c:v>
+                  <c:v>8677.2033333333329</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>8641.2380952380954</c:v>
+                  <c:v>8638.77</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>8596.7619047619046</c:v>
+                  <c:v>8589.5266666666666</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>8477.5714285714275</c:v>
+                  <c:v>8459.01</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>8473.7142857142862</c:v>
+                  <c:v>8497.5499999999993</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>8486.2857142857138</c:v>
+                  <c:v>8457.48</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>8411.4285714285725</c:v>
+                  <c:v>8432.119999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -22568,13 +22575,13 @@
     <xdr:from>
       <xdr:col>11</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>6</xdr:row>
+      <xdr:row>7</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
       <xdr:colOff>257175</xdr:colOff>
-      <xdr:row>30</xdr:row>
+      <xdr:row>31</xdr:row>
       <xdr:rowOff>109538</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -23189,10 +23196,10 @@
   <dimension ref="A1:BC63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="H3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A9" sqref="A9"/>
+      <selection pane="bottomRight" activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23660,8 +23667,8 @@
         <f>'weekly deaths'!AE15</f>
         <v>192</v>
       </c>
-      <c r="AF3" s="93"/>
-      <c r="AG3" s="93"/>
+      <c r="AF3" s="92"/>
+      <c r="AG3" s="92"/>
     </row>
     <row r="4" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A4" s="62" t="s">
@@ -23669,123 +23676,123 @@
       </c>
       <c r="B4" s="13">
         <f>SUM(C4:BB4)</f>
-        <v>301334.1428571429</v>
+        <v>300956.21999999991</v>
       </c>
       <c r="C4" s="13">
         <f>'step 3 - shift'!C4</f>
-        <v>13027.142857142857</v>
+        <v>13210.12</v>
       </c>
       <c r="D4" s="13">
         <f>'step 3 - shift'!D4</f>
-        <v>13600.285714285714</v>
+        <v>13491.96</v>
       </c>
       <c r="E4" s="13">
         <f>'step 3 - shift'!E4</f>
-        <v>12504</v>
+        <v>12388.98</v>
       </c>
       <c r="F4" s="13">
         <f>'step 3 - shift'!F4</f>
-        <v>11751.428571428572</v>
+        <v>11726.68</v>
       </c>
       <c r="G4" s="13">
         <f>'step 3 - shift'!G4</f>
-        <v>11343.714285714286</v>
+        <v>11280.22</v>
       </c>
       <c r="H4" s="13">
         <f>'step 3 - shift'!H4</f>
-        <v>10968</v>
+        <v>10963.740000000002</v>
       </c>
       <c r="I4" s="13">
         <f>'step 3 - shift'!I4</f>
-        <v>10899.857142857143</v>
+        <v>10889.41</v>
       </c>
       <c r="J4" s="13">
         <f>'step 3 - shift'!J4</f>
-        <v>10830.285714285714</v>
+        <v>10827.75</v>
       </c>
       <c r="K4" s="13">
         <f>'step 3 - shift'!K4</f>
-        <v>10849.857142857143</v>
+        <v>10857.869999999999</v>
       </c>
       <c r="L4" s="13">
         <f>'step 3 - shift'!L4</f>
-        <v>10946</v>
+        <v>10958.07</v>
       </c>
       <c r="M4" s="13">
         <f>'step 3 - shift'!M4</f>
-        <v>10811.714285714286</v>
+        <v>10763.84</v>
       </c>
       <c r="N4" s="13">
         <f>'step 3 - shift'!N4</f>
-        <v>10567.714285714286</v>
+        <v>10573.8</v>
       </c>
       <c r="O4" s="13">
         <f>'step 3 - shift'!O4</f>
-        <v>11592</v>
+        <v>11826.3</v>
       </c>
       <c r="P4" s="13">
         <f>'step 3 - shift'!P4</f>
-        <v>13239.642857142857</v>
+        <v>13317.184999999999</v>
       </c>
       <c r="Q4" s="13">
         <f>'step 3 - shift'!Q4</f>
-        <v>13712.285714285714</v>
+        <v>13720.755000000001</v>
       </c>
       <c r="R4" s="13">
         <f>'step 3 - shift'!R4</f>
-        <v>13319.857142857141</v>
+        <v>13215.69</v>
       </c>
       <c r="S4" s="13">
         <f>'step 3 - shift'!S4</f>
-        <v>12163.642857142859</v>
+        <v>12028.895</v>
       </c>
       <c r="T4" s="13">
         <f>'step 3 - shift'!T4</f>
-        <v>11003.714285714286</v>
+        <v>10908.861666666668</v>
       </c>
       <c r="U4" s="13">
         <f>'step 3 - shift'!U4</f>
-        <v>10097.380952380952</v>
+        <v>10009.352222222224</v>
       </c>
       <c r="V4" s="13">
         <f>'step 3 - shift'!V4</f>
-        <v>9394.3492063492067</v>
+        <v>9345.3366666666661</v>
       </c>
       <c r="W4" s="13">
         <f>'step 3 - shift'!W4</f>
-        <v>8941.5555555555566</v>
+        <v>8899.7444444444445</v>
       </c>
       <c r="X4" s="13">
         <f>'step 3 - shift'!X4</f>
-        <v>8682.7142857142844</v>
+        <v>8677.2033333333329</v>
       </c>
       <c r="Y4" s="13">
         <f>'step 3 - shift'!Y4</f>
-        <v>8641.2380952380954</v>
+        <v>8638.77</v>
       </c>
       <c r="Z4" s="13">
         <f>'step 3 - shift'!Z4</f>
-        <v>8596.7619047619046</v>
+        <v>8589.5266666666666</v>
       </c>
       <c r="AA4" s="13">
         <f>'step 3 - shift'!AA4</f>
-        <v>8477.5714285714275</v>
+        <v>8459.01</v>
       </c>
       <c r="AB4" s="13">
         <f>'step 3 - shift'!AB4</f>
-        <v>8473.7142857142862</v>
+        <v>8497.5499999999993</v>
       </c>
       <c r="AC4" s="13">
         <f>'step 3 - shift'!AC4</f>
-        <v>8486.2857142857138</v>
+        <v>8457.48</v>
       </c>
       <c r="AD4" s="13">
         <f>'step 3 - shift'!AD4</f>
-        <v>8411.4285714285725</v>
-      </c>
-      <c r="AE4" s="93"/>
-      <c r="AF4" s="93"/>
-      <c r="AG4" s="93"/>
+        <v>8432.119999999999</v>
+      </c>
+      <c r="AE4" s="92"/>
+      <c r="AF4" s="92"/>
+      <c r="AG4" s="92"/>
     </row>
     <row r="5" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A5" s="62" t="s">
@@ -23793,123 +23800,123 @@
       </c>
       <c r="B5" s="13">
         <f>SUM(C5:BB5)</f>
-        <v>352508.14285714284</v>
+        <v>352130.21999999991</v>
       </c>
       <c r="C5" s="13">
         <f t="shared" ref="C5:I5" si="0">C3+C4</f>
-        <v>13027.142857142857</v>
+        <v>13210.12</v>
       </c>
       <c r="D5" s="13">
         <f t="shared" si="0"/>
-        <v>13600.285714285714</v>
+        <v>13491.96</v>
       </c>
       <c r="E5" s="13">
         <f t="shared" si="0"/>
-        <v>12504</v>
+        <v>12388.98</v>
       </c>
       <c r="F5" s="13">
         <f t="shared" si="0"/>
-        <v>11751.428571428572</v>
+        <v>11726.68</v>
       </c>
       <c r="G5" s="13">
         <f t="shared" si="0"/>
-        <v>11343.714285714286</v>
+        <v>11280.22</v>
       </c>
       <c r="H5" s="13">
         <f t="shared" si="0"/>
-        <v>10968</v>
+        <v>10963.740000000002</v>
       </c>
       <c r="I5" s="13">
         <f t="shared" si="0"/>
-        <v>10899.857142857143</v>
+        <v>10889.41</v>
       </c>
       <c r="J5" s="13">
         <f>J3+J4</f>
-        <v>10830.285714285714</v>
+        <v>10827.75</v>
       </c>
       <c r="K5" s="13">
         <f t="shared" ref="K5:AD5" si="1">K3+K4</f>
-        <v>10849.857142857143</v>
-      </c>
-      <c r="L5" s="13">
+        <v>10857.869999999999</v>
+      </c>
+      <c r="L5" s="74">
         <f t="shared" si="1"/>
-        <v>10952</v>
-      </c>
-      <c r="M5" s="13">
+        <v>10964.07</v>
+      </c>
+      <c r="M5" s="74">
         <f t="shared" si="1"/>
-        <v>10855.714285714286</v>
-      </c>
-      <c r="N5" s="13">
+        <v>10807.84</v>
+      </c>
+      <c r="N5" s="74">
         <f t="shared" si="1"/>
-        <v>10968.714285714286</v>
-      </c>
-      <c r="O5" s="13">
+        <v>10974.8</v>
+      </c>
+      <c r="O5" s="74">
         <f t="shared" si="1"/>
-        <v>13463</v>
-      </c>
-      <c r="P5" s="13">
+        <v>13697.3</v>
+      </c>
+      <c r="P5" s="74">
         <f t="shared" si="1"/>
-        <v>18411.642857142855</v>
-      </c>
-      <c r="Q5" s="13">
+        <v>18489.184999999998</v>
+      </c>
+      <c r="Q5" s="74">
         <f t="shared" si="1"/>
-        <v>21926.285714285714</v>
-      </c>
-      <c r="R5" s="13">
+        <v>21934.755000000001</v>
+      </c>
+      <c r="R5" s="74">
         <f t="shared" si="1"/>
-        <v>21609.857142857141</v>
-      </c>
-      <c r="S5" s="13">
+        <v>21505.690000000002</v>
+      </c>
+      <c r="S5" s="74">
         <f t="shared" si="1"/>
-        <v>19078.642857142859</v>
-      </c>
-      <c r="T5" s="13">
+        <v>18943.895</v>
+      </c>
+      <c r="T5" s="74">
         <f t="shared" si="1"/>
-        <v>16187.714285714286</v>
-      </c>
-      <c r="U5" s="13">
+        <v>16092.861666666668</v>
+      </c>
+      <c r="U5" s="74">
         <f t="shared" si="1"/>
-        <v>14064.380952380952</v>
-      </c>
-      <c r="V5" s="13">
+        <v>13976.352222222224</v>
+      </c>
+      <c r="V5" s="74">
         <f t="shared" si="1"/>
-        <v>12245.349206349207</v>
-      </c>
-      <c r="W5" s="13">
+        <v>12196.336666666666</v>
+      </c>
+      <c r="W5" s="74">
         <f t="shared" si="1"/>
-        <v>11208.555555555557</v>
-      </c>
-      <c r="X5" s="13">
+        <v>11166.744444444445</v>
+      </c>
+      <c r="X5" s="74">
         <f t="shared" si="1"/>
-        <v>10452.714285714284</v>
-      </c>
-      <c r="Y5" s="13">
+        <v>10447.203333333333</v>
+      </c>
+      <c r="Y5" s="74">
         <f t="shared" si="1"/>
-        <v>9940.2380952380954</v>
-      </c>
-      <c r="Z5" s="13">
+        <v>9937.77</v>
+      </c>
+      <c r="Z5" s="74">
         <f t="shared" si="1"/>
-        <v>9531.7619047619046</v>
-      </c>
-      <c r="AA5" s="13">
+        <v>9524.5266666666666</v>
+      </c>
+      <c r="AA5" s="74">
         <f t="shared" si="1"/>
-        <v>9148.5714285714275</v>
-      </c>
-      <c r="AB5" s="13">
+        <v>9130.01</v>
+      </c>
+      <c r="AB5" s="74">
         <f t="shared" si="1"/>
-        <v>9045.7142857142862</v>
-      </c>
-      <c r="AC5" s="13">
+        <v>9069.5499999999993</v>
+      </c>
+      <c r="AC5" s="74">
         <f t="shared" si="1"/>
-        <v>8908.2857142857138</v>
-      </c>
-      <c r="AD5" s="13">
+        <v>8879.48</v>
+      </c>
+      <c r="AD5" s="74">
         <f t="shared" si="1"/>
-        <v>8734.4285714285725</v>
-      </c>
-      <c r="AE5" s="93"/>
-      <c r="AF5" s="93"/>
-      <c r="AG5" s="93"/>
+        <v>8755.119999999999</v>
+      </c>
+      <c r="AE5" s="92"/>
+      <c r="AF5" s="92"/>
+      <c r="AG5" s="92"/>
     </row>
     <row r="6" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A6" s="62" t="s">
@@ -23917,123 +23924,123 @@
       </c>
       <c r="B6" s="13">
         <f>SUM(C6:BB6)</f>
-        <v>57590.342857142859</v>
+        <v>57212.42</v>
       </c>
       <c r="C6" s="13">
         <f>C5-'weekly deaths'!C25</f>
-        <v>326.74285714285725</v>
+        <v>509.72000000000116</v>
       </c>
       <c r="D6" s="13">
         <f>D5-'weekly deaths'!D25</f>
-        <v>705.28571428571377</v>
+        <v>596.95999999999913</v>
       </c>
       <c r="E6" s="13">
         <f>E5-'weekly deaths'!E25</f>
-        <v>-114.60000000000036</v>
+        <v>-229.6200000000008</v>
       </c>
       <c r="F6" s="13">
         <f>F5-'weekly deaths'!F25</f>
-        <v>-421.97142857142717</v>
+        <v>-446.71999999999935</v>
       </c>
       <c r="G6" s="13">
         <f>G5-'weekly deaths'!G25</f>
-        <v>-735.88571428571413</v>
+        <v>-799.38000000000102</v>
       </c>
       <c r="H6" s="13">
         <f>H5-'weekly deaths'!H25</f>
-        <v>-702.79999999999927</v>
+        <v>-707.05999999999767</v>
       </c>
       <c r="I6" s="13">
         <f>I5-'weekly deaths'!I25</f>
-        <v>-760.74285714285725</v>
+        <v>-771.19000000000051</v>
       </c>
       <c r="J6" s="13">
         <f>J5-'weekly deaths'!J25</f>
-        <v>-572.11428571428587</v>
+        <v>-574.64999999999964</v>
       </c>
       <c r="K6" s="13">
         <f>K5-'weekly deaths'!K25</f>
-        <v>-473.34285714285761</v>
+        <v>-465.33000000000175</v>
       </c>
       <c r="L6" s="13">
         <f>L5-'weekly deaths'!L25</f>
-        <v>-300.79999999999927</v>
+        <v>-288.72999999999956</v>
       </c>
       <c r="M6" s="13">
         <f>M5-'weekly deaths'!M25</f>
-        <v>-54.285714285713766</v>
+        <v>-102.15999999999985</v>
       </c>
       <c r="N6" s="13">
         <f>N5-'weekly deaths'!N25</f>
-        <v>361.51428571428551</v>
+        <v>367.59999999999854</v>
       </c>
       <c r="O6" s="13">
         <f>O5-'weekly deaths'!O25</f>
-        <v>3014.2000000000007</v>
+        <v>3248.5</v>
       </c>
       <c r="P6" s="13">
         <f>P5-'weekly deaths'!P25</f>
-        <v>8051.2428571428554</v>
+        <v>8128.784999999998</v>
       </c>
       <c r="Q6" s="13">
         <f>Q5-'weekly deaths'!Q25</f>
-        <v>11662.885714285714</v>
+        <v>11671.355000000001</v>
       </c>
       <c r="R6" s="13">
         <f>R5-'weekly deaths'!R25</f>
-        <v>11525.057142857142</v>
+        <v>11420.890000000003</v>
       </c>
       <c r="S6" s="13">
         <f>S5-'weekly deaths'!S25</f>
-        <v>9266.442857142858</v>
+        <v>9131.6949999999997</v>
       </c>
       <c r="T6" s="13">
         <f>T5-'weekly deaths'!T25</f>
-        <v>6443.914285714287</v>
+        <v>6349.0616666666683</v>
       </c>
       <c r="U6" s="13">
         <f>U5-'weekly deaths'!U25</f>
-        <v>4318.3809523809523</v>
+        <v>4230.3522222222236</v>
       </c>
       <c r="V6" s="13">
         <f>V5-'weekly deaths'!V25</f>
-        <v>2708.3492063492067</v>
+        <v>2659.3366666666661</v>
       </c>
       <c r="W6" s="13">
         <f>W5-'weekly deaths'!W25</f>
-        <v>1708.3555555555558</v>
+        <v>1666.5444444444438</v>
       </c>
       <c r="X6" s="13">
         <f>X5-'weekly deaths'!X25</f>
-        <v>1255.7142857142844</v>
+        <v>1250.2033333333329</v>
       </c>
       <c r="Y6" s="13">
         <f>Y5-'weekly deaths'!Y25</f>
-        <v>716.83809523809578</v>
+        <v>714.3700000000008</v>
       </c>
       <c r="Z6" s="13">
         <f>Z5-'weekly deaths'!Z25</f>
-        <v>326.16190476190422</v>
+        <v>318.92666666666628</v>
       </c>
       <c r="AA6" s="13">
         <f>AA5-'weekly deaths'!AA25</f>
-        <v>-126.42857142857247</v>
+        <v>-144.98999999999978</v>
       </c>
       <c r="AB6" s="13">
         <f>AB5-'weekly deaths'!AB25</f>
-        <v>-5.8857142857141298</v>
+        <v>17.949999999998909</v>
       </c>
       <c r="AC6" s="13">
         <f>AC5-'weekly deaths'!AC25</f>
-        <v>-363.3142857142866</v>
+        <v>-392.1200000000008</v>
       </c>
       <c r="AD6" s="13">
         <f>AD5-'weekly deaths'!AD25</f>
-        <v>-168.57142857142753</v>
-      </c>
-      <c r="AE6" s="93"/>
-      <c r="AF6" s="93"/>
-      <c r="AG6" s="93"/>
+        <v>-147.88000000000102</v>
+      </c>
+      <c r="AE6" s="92"/>
+      <c r="AF6" s="92"/>
+      <c r="AG6" s="92"/>
     </row>
     <row r="7" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A7" s="62" t="s">
@@ -24041,78 +24048,78 @@
       </c>
       <c r="B7" s="13">
         <f>SUM(C7:BB7)</f>
-        <v>61359.057142857142</v>
-      </c>
-      <c r="C7" s="93"/>
-      <c r="D7" s="93"/>
-      <c r="E7" s="93"/>
-      <c r="F7" s="93"/>
-      <c r="G7" s="93"/>
-      <c r="H7" s="93"/>
-      <c r="I7" s="93"/>
-      <c r="J7" s="93"/>
-      <c r="K7" s="93"/>
-      <c r="L7" s="93"/>
-      <c r="M7" s="93"/>
+        <v>61157.62000000001</v>
+      </c>
+      <c r="C7" s="92"/>
+      <c r="D7" s="92"/>
+      <c r="E7" s="92"/>
+      <c r="F7" s="92"/>
+      <c r="G7" s="92"/>
+      <c r="H7" s="92"/>
+      <c r="I7" s="92"/>
+      <c r="J7" s="92"/>
+      <c r="K7" s="92"/>
+      <c r="L7" s="92"/>
+      <c r="M7" s="92"/>
       <c r="N7" s="13">
         <f>N6</f>
-        <v>361.51428571428551</v>
+        <v>367.59999999999854</v>
       </c>
       <c r="O7" s="13">
         <f t="shared" ref="O7:Z7" si="2">O6</f>
-        <v>3014.2000000000007</v>
+        <v>3248.5</v>
       </c>
       <c r="P7" s="13">
         <f t="shared" si="2"/>
-        <v>8051.2428571428554</v>
+        <v>8128.784999999998</v>
       </c>
       <c r="Q7" s="13">
         <f t="shared" si="2"/>
-        <v>11662.885714285714</v>
+        <v>11671.355000000001</v>
       </c>
       <c r="R7" s="13">
         <f t="shared" si="2"/>
-        <v>11525.057142857142</v>
+        <v>11420.890000000003</v>
       </c>
       <c r="S7" s="13">
         <f t="shared" si="2"/>
-        <v>9266.442857142858</v>
+        <v>9131.6949999999997</v>
       </c>
       <c r="T7" s="13">
         <f t="shared" si="2"/>
-        <v>6443.914285714287</v>
+        <v>6349.0616666666683</v>
       </c>
       <c r="U7" s="13">
         <f t="shared" si="2"/>
-        <v>4318.3809523809523</v>
+        <v>4230.3522222222236</v>
       </c>
       <c r="V7" s="13">
         <f t="shared" si="2"/>
-        <v>2708.3492063492067</v>
+        <v>2659.3366666666661</v>
       </c>
       <c r="W7" s="13">
         <f t="shared" si="2"/>
-        <v>1708.3555555555558</v>
+        <v>1666.5444444444438</v>
       </c>
       <c r="X7" s="13">
         <f t="shared" si="2"/>
-        <v>1255.7142857142844</v>
+        <v>1250.2033333333329</v>
       </c>
       <c r="Y7" s="13">
         <f t="shared" si="2"/>
-        <v>716.83809523809578</v>
+        <v>714.3700000000008</v>
       </c>
       <c r="Z7" s="13">
         <f t="shared" si="2"/>
-        <v>326.16190476190422</v>
-      </c>
-      <c r="AA7" s="93"/>
-      <c r="AB7" s="93"/>
-      <c r="AC7" s="93"/>
-      <c r="AD7" s="93"/>
-      <c r="AE7" s="93"/>
-      <c r="AF7" s="93"/>
-      <c r="AG7" s="93"/>
+        <v>318.92666666666628</v>
+      </c>
+      <c r="AA7" s="92"/>
+      <c r="AB7" s="92"/>
+      <c r="AC7" s="92"/>
+      <c r="AD7" s="92"/>
+      <c r="AE7" s="92"/>
+      <c r="AF7" s="92"/>
+      <c r="AG7" s="92"/>
     </row>
     <row r="63" spans="12:12" x14ac:dyDescent="0.25">
       <c r="L63" t="s">
@@ -24127,10 +24134,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79B149E2-77DB-41A2-80F6-2DEE02D8A44F}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -24148,18 +24155,21 @@
       <c r="A2" t="s">
         <v>40</v>
       </c>
-      <c r="B2" s="10">
-        <f>4/7</f>
-        <v>0.5714285714285714</v>
+      <c r="B2" s="94">
+        <v>0.47</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>41</v>
       </c>
-      <c r="B3" s="10">
-        <f>1-B2</f>
-        <v>0.4285714285714286</v>
+      <c r="B3" s="94">
+        <v>0.53</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -28609,7 +28619,7 @@
         <f t="shared" si="13"/>
         <v>43</v>
       </c>
-      <c r="J127" s="87">
+      <c r="J127" s="86">
         <f t="shared" si="11"/>
         <v>43.571428571428569</v>
       </c>
@@ -28643,7 +28653,7 @@
         <f t="shared" si="13"/>
         <v>54</v>
       </c>
-      <c r="J128" s="87">
+      <c r="J128" s="86">
         <f t="shared" si="11"/>
         <v>40.571428571428569</v>
       </c>
@@ -28677,28 +28687,28 @@
         <f t="shared" si="13"/>
         <v>40</v>
       </c>
-      <c r="J129" s="87">
+      <c r="J129" s="86">
         <f t="shared" si="11"/>
         <v>39</v>
       </c>
     </row>
     <row r="130" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A130" s="85">
+      <c r="A130" s="84">
         <v>44023</v>
       </c>
       <c r="B130" s="27">
         <v>41754</v>
       </c>
-      <c r="C130" s="91">
+      <c r="C130" s="90">
         <v>50971</v>
       </c>
       <c r="D130" s="27">
         <v>51177</v>
       </c>
-      <c r="E130" s="86">
+      <c r="E130" s="85">
         <v>51204</v>
       </c>
-      <c r="F130" s="92">
+      <c r="F130" s="91">
         <f t="shared" si="12"/>
         <v>2</v>
       </c>
@@ -28706,33 +28716,33 @@
         <f t="shared" si="10"/>
         <v>50</v>
       </c>
-      <c r="H130" s="88"/>
-      <c r="I130" s="87">
+      <c r="H130" s="87"/>
+      <c r="I130" s="86">
         <f t="shared" si="13"/>
         <v>30</v>
       </c>
-      <c r="J130" s="87">
+      <c r="J130" s="86">
         <f t="shared" si="11"/>
         <v>37.428571428571431</v>
       </c>
     </row>
     <row r="131" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A131" s="85">
+      <c r="A131" s="84">
         <v>44024</v>
       </c>
       <c r="B131" s="27">
         <v>41754</v>
       </c>
-      <c r="C131" s="91">
+      <c r="C131" s="90">
         <v>50971</v>
       </c>
       <c r="D131" s="27">
         <v>51200</v>
       </c>
-      <c r="E131" s="86">
+      <c r="E131" s="85">
         <v>51231</v>
       </c>
-      <c r="F131" s="92">
+      <c r="F131" s="91">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
@@ -28740,33 +28750,33 @@
         <f t="shared" si="10"/>
         <v>46.428571428571431</v>
       </c>
-      <c r="H131" s="88"/>
-      <c r="I131" s="87">
+      <c r="H131" s="87"/>
+      <c r="I131" s="86">
         <f t="shared" si="13"/>
         <v>27</v>
       </c>
-      <c r="J131" s="87">
+      <c r="J131" s="86">
         <f t="shared" si="11"/>
         <v>35.714285714285715</v>
       </c>
     </row>
     <row r="132" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A132" s="85">
+      <c r="A132" s="84">
         <v>44025</v>
       </c>
       <c r="B132" s="27">
         <v>41754</v>
       </c>
-      <c r="C132" s="91">
+      <c r="C132" s="90">
         <v>51034</v>
       </c>
       <c r="D132" s="27">
         <v>51233</v>
       </c>
-      <c r="E132" s="86">
+      <c r="E132" s="85">
         <v>51268</v>
       </c>
-      <c r="F132" s="92">
+      <c r="F132" s="91">
         <f t="shared" si="12"/>
         <v>63</v>
       </c>
@@ -28774,33 +28784,33 @@
         <f t="shared" si="10"/>
         <v>44.285714285714285</v>
       </c>
-      <c r="H132" s="88"/>
-      <c r="I132" s="87">
+      <c r="H132" s="87"/>
+      <c r="I132" s="86">
         <f t="shared" si="13"/>
         <v>37</v>
       </c>
-      <c r="J132" s="87">
+      <c r="J132" s="86">
         <f t="shared" si="11"/>
         <v>30.285714285714285</v>
       </c>
     </row>
     <row r="133" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A133" s="85">
+      <c r="A133" s="84">
         <v>44026</v>
       </c>
       <c r="B133" s="27">
         <v>41754</v>
       </c>
-      <c r="C133" s="91">
+      <c r="C133" s="90">
         <v>51102</v>
       </c>
       <c r="D133" s="27">
         <v>51256</v>
       </c>
-      <c r="E133" s="86">
+      <c r="E133" s="85">
         <v>51299</v>
       </c>
-      <c r="F133" s="92">
+      <c r="F133" s="91">
         <f t="shared" si="12"/>
         <v>68</v>
       </c>
@@ -28808,99 +28818,99 @@
         <f t="shared" si="10"/>
         <v>42.142857142857146</v>
       </c>
-      <c r="H133" s="88"/>
-      <c r="I133" s="87">
+      <c r="H133" s="87"/>
+      <c r="I133" s="86">
         <f t="shared" si="13"/>
         <v>31</v>
       </c>
-      <c r="J133" s="87">
+      <c r="J133" s="86">
         <f t="shared" si="11"/>
         <v>27.428571428571427</v>
       </c>
     </row>
     <row r="134" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A134" s="85">
+      <c r="A134" s="84">
         <v>44027</v>
       </c>
       <c r="B134" s="27">
         <v>41754</v>
       </c>
-      <c r="C134" s="91">
+      <c r="C134" s="90">
         <v>51160</v>
       </c>
       <c r="D134" s="27">
         <v>51269</v>
       </c>
-      <c r="E134" s="86">
+      <c r="E134" s="85">
         <v>51330</v>
       </c>
-      <c r="F134" s="92">
+      <c r="F134" s="91">
         <f t="shared" si="12"/>
         <v>58</v>
       </c>
-      <c r="G134" s="88"/>
-      <c r="H134" s="88"/>
-      <c r="I134" s="87">
+      <c r="G134" s="87"/>
+      <c r="H134" s="87"/>
+      <c r="I134" s="86">
         <f t="shared" si="13"/>
         <v>31</v>
       </c>
-      <c r="J134" s="88"/>
+      <c r="J134" s="87"/>
     </row>
     <row r="135" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A135" s="85">
+      <c r="A135" s="84">
         <v>44028</v>
       </c>
       <c r="B135" s="27">
         <v>41754</v>
       </c>
-      <c r="C135" s="91">
+      <c r="C135" s="90">
         <v>51215</v>
       </c>
       <c r="D135" s="27">
         <v>51277</v>
       </c>
-      <c r="E135" s="86">
+      <c r="E135" s="85">
         <v>51346</v>
       </c>
-      <c r="F135" s="92">
+      <c r="F135" s="91">
         <f t="shared" si="12"/>
         <v>55</v>
       </c>
-      <c r="G135" s="88"/>
-      <c r="H135" s="88"/>
-      <c r="I135" s="87">
+      <c r="G135" s="87"/>
+      <c r="H135" s="87"/>
+      <c r="I135" s="86">
         <f t="shared" si="13"/>
         <v>16</v>
       </c>
-      <c r="J135" s="88"/>
+      <c r="J135" s="87"/>
     </row>
     <row r="136" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A136" s="85">
+      <c r="A136" s="84">
         <v>44029</v>
       </c>
       <c r="B136" s="27">
         <v>41754</v>
       </c>
-      <c r="C136" s="91">
+      <c r="C136" s="90">
         <v>51264</v>
       </c>
       <c r="D136" s="27">
         <v>51277</v>
       </c>
-      <c r="E136" s="86">
+      <c r="E136" s="85">
         <v>51366</v>
       </c>
-      <c r="F136" s="92">
+      <c r="F136" s="91">
         <f t="shared" si="12"/>
         <v>49</v>
       </c>
-      <c r="G136" s="88"/>
-      <c r="H136" s="88"/>
-      <c r="I136" s="87">
+      <c r="G136" s="87"/>
+      <c r="H136" s="87"/>
+      <c r="I136" s="86">
         <f t="shared" si="13"/>
         <v>20</v>
       </c>
-      <c r="J136" s="88"/>
+      <c r="J136" s="87"/>
     </row>
     <row r="137" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B137"/>
@@ -28912,7 +28922,7 @@
       <c r="J137" s="31"/>
     </row>
     <row r="138" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A138" s="90" t="s">
+      <c r="A138" s="89" t="s">
         <v>42</v>
       </c>
       <c r="B138"/>
@@ -29093,10 +29103,10 @@
   <dimension ref="A1:CQ25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="W3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="AE18" sqref="AE18"/>
+      <selection pane="bottomRight" activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -30669,7 +30679,9 @@
       <c r="A18" s="62" t="s">
         <v>38</v>
       </c>
-      <c r="B18" s="13"/>
+      <c r="B18" s="13" t="s">
+        <v>45</v>
+      </c>
       <c r="C18" s="76"/>
       <c r="D18" s="76"/>
       <c r="E18" s="76"/>
@@ -30681,83 +30693,83 @@
       <c r="K18" s="76"/>
       <c r="L18" s="13">
         <f>params!$B2*L13+params!$B3*M13</f>
-        <v>2.1428571428571432</v>
+        <v>2.6500000000000004</v>
       </c>
       <c r="M18" s="13">
         <f>params!$B2*M13+params!$B3*N13</f>
-        <v>47</v>
+        <v>56.940000000000005</v>
       </c>
       <c r="N18" s="13">
         <f>params!$B2*N13+params!$B3*O13</f>
-        <v>289.85714285714289</v>
+        <v>334.08000000000004</v>
       </c>
       <c r="O18" s="13">
         <f>params!$B2*O13+params!$B3*P13</f>
-        <v>1797.2857142857144</v>
+        <v>2095.08</v>
       </c>
       <c r="P18" s="13">
         <f>params!$B2*P13+params!$B3*Q13</f>
-        <v>4648.4285714285716</v>
+        <v>4926.1400000000003</v>
       </c>
       <c r="Q18" s="13">
         <f>params!$B2*Q13+params!$B3*R13</f>
-        <v>7303.7142857142862</v>
+        <v>7561.8499999999995</v>
       </c>
       <c r="R18" s="13">
         <f>params!$B2*R13+params!$B3*S13</f>
-        <v>8534.7142857142862</v>
+        <v>8481.8700000000008</v>
       </c>
       <c r="S18" s="13">
         <f>params!$B2*S13+params!$B3*T13</f>
-        <v>7293.2857142857138</v>
+        <v>7069.9400000000005</v>
       </c>
       <c r="T18" s="13">
         <f>params!$B2*T13+params!$B3*U13</f>
-        <v>5132.8571428571431</v>
+        <v>4919.3500000000004</v>
       </c>
       <c r="U18" s="13">
         <f>params!$B2*U13+params!$B3*V13</f>
-        <v>3878.5714285714284</v>
+        <v>3866.4</v>
       </c>
       <c r="V18" s="13">
         <f>params!$B2*V13+params!$B3*W13</f>
-        <v>3286.7142857142853</v>
+        <v>3162.87</v>
       </c>
       <c r="W18" s="13">
         <f>params!$B2*W13+params!$B3*X13</f>
-        <v>2260.2857142857142</v>
+        <v>2182.4899999999998</v>
       </c>
       <c r="X18" s="13">
         <f>params!$B2*X13+params!$B3*Y13</f>
-        <v>1721.7142857142858</v>
+        <v>1697.98</v>
       </c>
       <c r="Y18" s="13">
         <f>params!$B2*Y13+params!$B3*Z13</f>
-        <v>1384.8571428571427</v>
+        <v>1336.7800000000002</v>
       </c>
       <c r="Z18" s="13">
         <f>params!$B2*Z13+params!$B3*AA13</f>
-        <v>972.14285714285711</v>
+        <v>938.56999999999994</v>
       </c>
       <c r="AA18" s="13">
         <f>params!$B2*AA13+params!$B3*AB13</f>
-        <v>707.14285714285711</v>
+        <v>689.19</v>
       </c>
       <c r="AB18" s="13">
         <f>params!$B2*AB13+params!$B3*AC13</f>
-        <v>574.28571428571433</v>
+        <v>566.78</v>
       </c>
       <c r="AC18" s="13">
         <f>params!$B2*AC13+params!$B3*AD13</f>
-        <v>460.85714285714289</v>
+        <v>444.02</v>
       </c>
       <c r="AD18" s="13">
         <f>params!$B2*AD13+params!$B3*AE13</f>
-        <v>335.57142857142856</v>
+        <v>328.37</v>
       </c>
       <c r="AE18" s="82">
         <f>params!$B2*AE13+params!$B3*AF13</f>
-        <v>168.57142857142856</v>
+        <v>138.65</v>
       </c>
       <c r="AF18" s="76"/>
       <c r="AG18" s="76"/>
@@ -31718,7 +31730,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FF79277-DA21-43EE-B272-D2265A09C468}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="M26" sqref="M26"/>
     </sheetView>
   </sheetViews>
@@ -31737,7 +31749,7 @@
       <pane xSplit="2" ySplit="2" topLeftCell="J3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="AE3" sqref="AE3"/>
+      <selection pane="bottomRight" activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -32289,13 +32301,13 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FC75FE2-1E89-4FAE-9623-041E358FEFA0}">
-  <dimension ref="A1:BC5"/>
+  <dimension ref="A1:BC6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="I3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="AE3" sqref="AE3"/>
+      <selection pane="bottomRight" activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -32763,26 +32775,26 @@
         <f>'step 1 - non-covid'!AE3</f>
         <v>8528</v>
       </c>
-      <c r="AF3" s="94"/>
-      <c r="AG3" s="94"/>
+      <c r="AF3" s="93"/>
+      <c r="AG3" s="93"/>
     </row>
     <row r="4" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A4" s="62" t="s">
         <v>35</v>
       </c>
       <c r="B4" s="12"/>
-      <c r="C4" s="94"/>
-      <c r="D4" s="94"/>
-      <c r="E4" s="94"/>
-      <c r="F4" s="94"/>
-      <c r="G4" s="94"/>
-      <c r="H4" s="94"/>
-      <c r="I4" s="94"/>
-      <c r="J4" s="94"/>
-      <c r="K4" s="94"/>
-      <c r="L4" s="94"/>
-      <c r="M4" s="94"/>
-      <c r="N4" s="94"/>
+      <c r="C4" s="93"/>
+      <c r="D4" s="93"/>
+      <c r="E4" s="93"/>
+      <c r="F4" s="93"/>
+      <c r="G4" s="93"/>
+      <c r="H4" s="93"/>
+      <c r="I4" s="93"/>
+      <c r="J4" s="93"/>
+      <c r="K4" s="93"/>
+      <c r="L4" s="93"/>
+      <c r="M4" s="93"/>
+      <c r="N4" s="93"/>
       <c r="O4" s="80"/>
       <c r="P4" s="80"/>
       <c r="Q4" s="79">
@@ -32816,13 +32828,13 @@
         <v>234.66666666666666</v>
       </c>
       <c r="Z4" s="80"/>
-      <c r="AA4" s="94"/>
-      <c r="AB4" s="94"/>
-      <c r="AC4" s="94"/>
-      <c r="AD4" s="94"/>
-      <c r="AE4" s="94"/>
-      <c r="AF4" s="94"/>
-      <c r="AG4" s="94"/>
+      <c r="AA4" s="93"/>
+      <c r="AB4" s="93"/>
+      <c r="AC4" s="93"/>
+      <c r="AD4" s="93"/>
+      <c r="AE4" s="93"/>
+      <c r="AF4" s="93"/>
+      <c r="AG4" s="93"/>
     </row>
     <row r="5" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A5" s="62" t="s">
@@ -32948,8 +32960,17 @@
         <f t="shared" si="0"/>
         <v>8528</v>
       </c>
-      <c r="AF5" s="94"/>
-      <c r="AG5" s="94"/>
+      <c r="AF5" s="93"/>
+      <c r="AG5" s="93"/>
+    </row>
+    <row r="6" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="A6" s="62" t="s">
+        <v>43</v>
+      </c>
+      <c r="B6" s="13">
+        <f>B3-B5</f>
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -32962,10 +32983,10 @@
   <dimension ref="A1:BC6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="J3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="AE3" sqref="AE3"/>
+      <selection pane="bottomRight" activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -33433,8 +33454,8 @@
         <f>'step 2 - smooth'!AE5</f>
         <v>8528</v>
       </c>
-      <c r="AF3" s="93"/>
-      <c r="AG3" s="93"/>
+      <c r="AF3" s="92"/>
+      <c r="AG3" s="92"/>
     </row>
     <row r="4" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A4" s="62" t="s">
@@ -33442,135 +33463,135 @@
       </c>
       <c r="B4" s="13">
         <f>SUM(C4:BC4)</f>
-        <v>301334.1428571429</v>
+        <v>300956.21999999991</v>
       </c>
       <c r="C4" s="13">
         <f>params!$B2*C3+params!$B3*D3</f>
-        <v>13027.142857142857</v>
+        <v>13210.12</v>
       </c>
       <c r="D4" s="13">
         <f>params!$B2*D3+params!$B3*E3</f>
-        <v>13600.285714285714</v>
+        <v>13491.96</v>
       </c>
       <c r="E4" s="13">
         <f>params!$B2*E3+params!$B3*F3</f>
-        <v>12504</v>
+        <v>12388.98</v>
       </c>
       <c r="F4" s="13">
         <f>params!$B2*F3+params!$B3*G3</f>
-        <v>11751.428571428572</v>
+        <v>11726.68</v>
       </c>
       <c r="G4" s="13">
         <f>params!$B2*G3+params!$B3*H3</f>
-        <v>11343.714285714286</v>
+        <v>11280.22</v>
       </c>
       <c r="H4" s="13">
         <f>params!$B2*H3+params!$B3*I3</f>
-        <v>10968</v>
+        <v>10963.740000000002</v>
       </c>
       <c r="I4" s="13">
         <f>params!$B2*I3+params!$B3*J3</f>
-        <v>10899.857142857143</v>
+        <v>10889.41</v>
       </c>
       <c r="J4" s="13">
         <f>params!$B2*J3+params!$B3*K3</f>
-        <v>10830.285714285714</v>
+        <v>10827.75</v>
       </c>
       <c r="K4" s="13">
         <f>params!$B2*K3+params!$B3*L3</f>
-        <v>10849.857142857143</v>
+        <v>10857.869999999999</v>
       </c>
       <c r="L4" s="13">
         <f>params!$B2*L3+params!$B3*M3</f>
-        <v>10946</v>
+        <v>10958.07</v>
       </c>
       <c r="M4" s="13">
         <f>params!$B2*M3+params!$B3*N3</f>
-        <v>10811.714285714286</v>
+        <v>10763.84</v>
       </c>
       <c r="N4" s="13">
         <f>params!$B2*N3+params!$B3*O3</f>
-        <v>10567.714285714286</v>
+        <v>10573.8</v>
       </c>
       <c r="O4" s="13">
         <f>params!$B2*O3+params!$B3*P3</f>
-        <v>11592</v>
+        <v>11826.3</v>
       </c>
       <c r="P4" s="13">
         <f>params!$B2*P3+params!$B3*Q3</f>
-        <v>13239.642857142857</v>
+        <v>13317.184999999999</v>
       </c>
       <c r="Q4" s="79">
         <f>params!$B2*Q3+params!$B3*R3</f>
-        <v>13712.285714285714</v>
+        <v>13720.755000000001</v>
       </c>
       <c r="R4" s="79">
         <f>params!$B2*R3+params!$B3*S3</f>
-        <v>13319.857142857141</v>
+        <v>13215.69</v>
       </c>
       <c r="S4" s="74">
         <f>params!$B2*S3+params!$B3*T3</f>
-        <v>12163.642857142859</v>
+        <v>12028.895</v>
       </c>
       <c r="T4" s="13">
         <f>params!$B2*T3+params!$B3*U3</f>
-        <v>11003.714285714286</v>
+        <v>10908.861666666668</v>
       </c>
       <c r="U4" s="79">
         <f>params!$B2*U3+params!$B3*V3</f>
-        <v>10097.380952380952</v>
+        <v>10009.352222222224</v>
       </c>
       <c r="V4" s="74">
         <f>params!$B2*V3+params!$B3*W3</f>
-        <v>9394.3492063492067</v>
+        <v>9345.3366666666661</v>
       </c>
       <c r="W4" s="13">
         <f>params!$B2*W3+params!$B3*X3</f>
-        <v>8941.5555555555566</v>
+        <v>8899.7444444444445</v>
       </c>
       <c r="X4" s="79">
         <f>params!$B2*X3+params!$B3*Y3</f>
-        <v>8682.7142857142844</v>
+        <v>8677.2033333333329</v>
       </c>
       <c r="Y4" s="74">
         <f>params!$B2*Y3+params!$B3*Z3</f>
-        <v>8641.2380952380954</v>
+        <v>8638.77</v>
       </c>
       <c r="Z4" s="13">
         <f>params!$B2*Z3+params!$B3*AA3</f>
-        <v>8596.7619047619046</v>
+        <v>8589.5266666666666</v>
       </c>
       <c r="AA4" s="13">
         <f>params!$B2*AA3+params!$B3*AB3</f>
-        <v>8477.5714285714275</v>
+        <v>8459.01</v>
       </c>
       <c r="AB4" s="13">
         <f>params!$B2*AB3+params!$B3*AC3</f>
-        <v>8473.7142857142862</v>
+        <v>8497.5499999999993</v>
       </c>
       <c r="AC4" s="13">
         <f>params!$B2*AC3+params!$B3*AD3</f>
-        <v>8486.2857142857138</v>
+        <v>8457.48</v>
       </c>
       <c r="AD4" s="13">
         <f>params!$B2*AD3+params!$B3*AE3</f>
-        <v>8411.4285714285725</v>
-      </c>
-      <c r="AE4" s="93"/>
-      <c r="AF4" s="93"/>
-      <c r="AG4" s="93"/>
+        <v>8432.119999999999</v>
+      </c>
+      <c r="AE4" s="92"/>
+      <c r="AF4" s="92"/>
+      <c r="AG4" s="92"/>
     </row>
     <row r="5" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="A5" s="81" t="s">
+      <c r="A5" s="62" t="s">
         <v>43</v>
       </c>
-      <c r="B5" s="84">
-        <f>B3-B4-params!B3*C3</f>
-        <v>4873.142857142815</v>
+      <c r="B5" s="13">
+        <f>B3-B4-params!B3*C3-params!B2*AE3</f>
+        <v>8.6401996668428183E-11</v>
       </c>
     </row>
     <row r="6" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="B6" s="89"/>
+      <c r="B6" s="88"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Commit latest copy of 2020 weekly deaths
</commit_message>
<xml_diff>
--- a/data/ons_weekly_deaths_2020.xlsx
+++ b/data/ons_weekly_deaths_2020.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\WCA\ons-stats\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AAB7A10-D4E8-4638-8E1D-0C8F8CFCDAA2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7F3F12E-C917-4F06-BBFE-C03846D2AD8F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="748" activeTab="9" xr2:uid="{2E10C76F-872B-452C-8A27-924470753E43}"/>
   </bookViews>
@@ -5336,165 +5336,8 @@
           </c:extLst>
         </c:ser>
         <c:ser>
-          <c:idx val="1"/>
+          <c:idx val="3"/>
           <c:order val="1"/>
-          <c:tx>
-            <c:v>5-Year Average</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:srgbClr val="00B050"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>'step 4 - combine'!$L$2:$AD$2</c:f>
-              <c:numCache>
-                <c:formatCode>d\-mmm\-yy</c:formatCode>
-                <c:ptCount val="19"/>
-                <c:pt idx="0">
-                  <c:v>43896</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>43903</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>43910</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>43917</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>43924</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>43931</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>43938</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>43945</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>43952</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>43959</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>43966</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>43973</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>43980</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>43987</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>43994</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>44001</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>44008</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>44015</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>44022</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'weekly deaths'!$L$25:$AD$25</c:f>
-              <c:numCache>
-                <c:formatCode>0</c:formatCode>
-                <c:ptCount val="19"/>
-                <c:pt idx="0">
-                  <c:v>11252.8</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>10910</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>10607.2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>10448.799999999999</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>10360.4</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>10263.4</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>10084.799999999999</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>9812.2000000000007</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>9743.7999999999993</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>9746</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>9537</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>9500.2000000000007</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>9197</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>9223.4</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>9205.6</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>9275</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>9051.6</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>9271.6</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>8903</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-E66F-4ACE-AE81-ED96FF0A843E}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="2"/>
           <c:tx>
             <c:v>Weekly deaths where COVID-19 was mentioned on the death certificate</c:v>
           </c:tx>
@@ -6365,994 +6208,6 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-5CE0-4794-9870-32BB32A7CB78}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:v>Weekly deaths where COVID-19 was mentioned on the death certificate</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>'step 4 - combine'!$C$2:$AD$2</c:f>
-              <c:numCache>
-                <c:formatCode>d\-mmm\-yy</c:formatCode>
-                <c:ptCount val="28"/>
-                <c:pt idx="0">
-                  <c:v>43833</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>43840</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>43847</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>43854</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>43861</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>43868</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>43875</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>43882</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>43889</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>43896</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>43903</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>43910</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>43917</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>43924</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>43931</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>43938</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>43945</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>43952</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>43959</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>43966</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>43973</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>43980</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>43987</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>43994</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>44001</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>44008</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>44015</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>44022</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'step 4 - combine'!$C$3:$AD$3</c:f>
-              <c:numCache>
-                <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="28"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>44</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>401</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>1871</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>5172</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>8214</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>8290</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>6915</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>5184</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>3967</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>2851</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>2267</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>1770</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>1299</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>935</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>671</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>572</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>422</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>323</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-5CE0-4794-9870-32BB32A7CB78}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:smooth val="0"/>
-        <c:axId val="693274200"/>
-        <c:axId val="693275184"/>
-      </c:lineChart>
-      <c:dateAx>
-        <c:axId val="693274200"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:numFmt formatCode="d\-mmm\-yy" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="693275184"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblOffset val="100"/>
-        <c:baseTimeUnit val="days"/>
-      </c:dateAx>
-      <c:valAx>
-        <c:axId val="693275184"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="#,##0" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="693274200"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="t"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart14.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-GB"/>
-              <a:t>Weekly death registrations for</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-GB" baseline="0"/>
-              <a:t> all causes and </a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-GB" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
-                <a:effectLst/>
-              </a:rPr>
-              <a:t>COVID-19</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-GB"/>
-          </a:p>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-GB"/>
-              <a:t>Source: Office for National Statistics,</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-GB" baseline="0"/>
-              <a:t> weekly </a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-GB"/>
-              <a:t>data released on 28th July</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:v>Weekly Registrations</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="25400" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:prstDash val="sysDash"/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>'weekly deaths'!$L$2:$AD$2</c:f>
-              <c:numCache>
-                <c:formatCode>d\-mmm\-yy</c:formatCode>
-                <c:ptCount val="19"/>
-                <c:pt idx="0">
-                  <c:v>43896</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>43903</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>43910</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>43917</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>43924</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>43931</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>43938</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>43945</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>43952</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>43959</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>43966</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>43973</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>43980</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>43987</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>43994</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>44001</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>44008</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>44015</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>44022</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'weekly deaths'!$L$3:$AD$3</c:f>
-              <c:numCache>
-                <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="19"/>
-                <c:pt idx="0">
-                  <c:v>10895</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>11019</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>10645</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>11141</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>16387</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>18516</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>22351</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>21997</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>17953</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>12657</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>14573</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>12288</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>9824</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>10709</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>9976</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>9339</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>8979</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>9140</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>8690</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-8214-4D9F-A8F4-6EDC2D9134EA}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:v>5-Year Average</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:srgbClr val="00B050"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>'weekly deaths'!$L$2:$AD$2</c:f>
-              <c:numCache>
-                <c:formatCode>d\-mmm\-yy</c:formatCode>
-                <c:ptCount val="19"/>
-                <c:pt idx="0">
-                  <c:v>43896</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>43903</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>43910</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>43917</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>43924</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>43931</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>43938</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>43945</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>43952</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>43959</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>43966</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>43973</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>43980</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>43987</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>43994</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>44001</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>44008</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>44015</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>44022</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'weekly deaths'!$L$5:$AD$5</c:f>
-              <c:numCache>
-                <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="19"/>
-                <c:pt idx="0">
-                  <c:v>11498</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>11205</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>10573</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>10130</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>10305</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>10520</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>10497</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>10458</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>9941</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>9576</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>10188</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>9940</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>8171</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>9977</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>9417</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>9404</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>9293</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>9183</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>9250</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-8214-4D9F-A8F4-6EDC2D9134EA}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:v>Weekly Registrations where COVID-19 was mentioned on the death certificate</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-              <a:prstDash val="sysDash"/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>'weekly deaths'!$L$2:$AD$2</c:f>
-              <c:numCache>
-                <c:formatCode>d\-mmm\-yy</c:formatCode>
-                <c:ptCount val="19"/>
-                <c:pt idx="0">
-                  <c:v>43896</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>43903</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>43910</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>43917</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>43924</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>43931</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>43938</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>43945</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>43952</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>43959</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>43966</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>43973</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>43980</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>43987</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>43994</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>44001</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>44008</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>44015</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>44022</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'weekly deaths'!$L$13:$AD$13</c:f>
-              <c:numCache>
-                <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="19"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>103</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>539</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>3475</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6213</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>8758</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>8237</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>6035</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>3930</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>3810</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>2589</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>1822</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>1588</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>1114</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>783</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>606</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>532</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>366</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-8214-4D9F-A8F4-6EDC2D9134EA}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -14704,46 +13559,6 @@
 </cs:colorStyle>
 </file>
 
-<file path=xl/charts/colors14.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
 <file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -17129,522 +15944,6 @@
 </file>
 
 <file path=xl/charts/style13.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="28575" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
-<file path=xl/charts/style14.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -22809,44 +21108,6 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>61</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>409575</xdr:colOff>
-      <xdr:row>85</xdr:row>
-      <xdr:rowOff>109538</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="6" name="Chart 5">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{86FDB196-0D1D-403F-87AB-AF757C7B6C26}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr>
-          <a:graphicFrameLocks/>
-        </xdr:cNvGraphicFramePr>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -23196,7 +21457,7 @@
   <dimension ref="A1:BC63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="H3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C24" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
       <selection pane="bottomRight" activeCell="A10" sqref="A10"/>
@@ -31730,7 +29991,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FF79277-DA21-43EE-B272-D2265A09C468}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M26" sqref="M26"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Tweak colours on graphs
</commit_message>
<xml_diff>
--- a/data/ons_weekly_deaths_2020.xlsx
+++ b/data/ons_weekly_deaths_2020.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\WCA\ons-stats\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7F3F12E-C917-4F06-BBFE-C03846D2AD8F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{510033EB-19C0-435E-84FE-D15FD0AFFA9E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="748" activeTab="9" xr2:uid="{2E10C76F-872B-452C-8A27-924470753E43}"/>
   </bookViews>
@@ -12366,15 +12366,12 @@
           <c:idx val="0"/>
           <c:order val="1"/>
           <c:tx>
-            <c:v>Weekly Trend</c:v>
+            <c:v>Weekly Trend - Affected by Bank Holidays</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent1">
-                  <a:lumMod val="60000"/>
-                  <a:lumOff val="40000"/>
-                </a:schemeClr>
+                <a:srgbClr val="C00000"/>
               </a:solidFill>
               <a:prstDash val="sysDash"/>
               <a:round/>
@@ -12386,22 +12383,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'step 2 - smooth'!$L$3:$AD$3</c:f>
+              <c:f>'step 1 - non-covid'!$L$4:$AD$4</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="19"/>
-                <c:pt idx="0">
-                  <c:v>10895</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>11014</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>10542</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>10602</c:v>
-                </c:pt>
                 <c:pt idx="4">
                   <c:v>12912</c:v>
                 </c:pt>
@@ -12434,18 +12419,6 @@
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>8862</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>8556</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>8373</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>8608</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>8324</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -13004,7 +12977,7 @@
           <c:idx val="0"/>
           <c:order val="1"/>
           <c:tx>
-            <c:v>Non-COVID deaths (occurences)</c:v>
+            <c:v>Non-COVID deaths (occurrences)</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
@@ -21457,7 +21430,7 @@
   <dimension ref="A1:BC63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C24" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
       <selection pane="bottomRight" activeCell="A10" sqref="A10"/>
@@ -30010,7 +29983,7 @@
       <pane xSplit="2" ySplit="2" topLeftCell="J3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="J6" sqref="J6"/>
+      <selection pane="bottomRight" activeCell="K32" sqref="K32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -30568,7 +30541,7 @@
       <pane xSplit="2" ySplit="2" topLeftCell="I3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A8" sqref="A8"/>
+      <selection pane="bottomRight" activeCell="S34" sqref="S34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -31247,7 +31220,7 @@
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A7" sqref="A7"/>
+      <selection pane="bottomRight" activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>